<commit_message>
Updated habitat quality data to include AU Step 1 priorities
previously the AU priorities in the protection data were restoration scores, not protection scores (for AU Step 1 priorities)
</commit_message>
<xml_diff>
--- a/Protection/habitat_quality_scores.xlsx
+++ b/Protection/habitat_quality_scores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3875" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3821" uniqueCount="894">
   <si>
     <t>ReachName</t>
   </si>
@@ -3251,7 +3251,7 @@
         <v>890</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -3328,7 +3328,7 @@
         <v>890</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -3408,7 +3408,7 @@
         <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -3491,7 +3491,7 @@
         <v>890</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -3568,7 +3568,7 @@
         <v>890</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -3648,7 +3648,7 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>5</v>
@@ -3728,7 +3728,7 @@
         <v>890</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -3814,7 +3814,7 @@
         <v>890</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -3903,7 +3903,7 @@
         <v>2</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -3986,7 +3986,7 @@
         <v>890</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -4072,7 +4072,7 @@
         <v>890</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -4158,7 +4158,7 @@
         <v>890</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -4416,7 +4416,7 @@
         <v>890</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -4493,7 +4493,7 @@
         <v>890</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -4573,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>5</v>
@@ -4659,7 +4659,7 @@
         <v>2</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>5</v>
@@ -4745,7 +4745,7 @@
         <v>2</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>5</v>
@@ -5089,7 +5089,7 @@
         <v>2</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>5</v>
@@ -5430,10 +5430,10 @@
         <v>890</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29">
         <v>5</v>
@@ -5516,7 +5516,7 @@
         <v>890</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H30">
         <v>2</v>
@@ -5937,10 +5937,10 @@
         <v>890</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35">
         <v>5</v>
@@ -6023,10 +6023,10 @@
         <v>890</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I36">
         <v>5</v>
@@ -6195,7 +6195,7 @@
         <v>890</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H38">
         <v>2</v>
@@ -6453,7 +6453,7 @@
         <v>890</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -6539,10 +6539,10 @@
         <v>890</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42">
         <v>5</v>
@@ -6714,7 +6714,7 @@
         <v>3</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I44">
         <v>5</v>
@@ -6800,7 +6800,7 @@
         <v>3</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I45">
         <v>5</v>
@@ -6969,7 +6969,7 @@
         <v>890</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -7046,7 +7046,7 @@
         <v>890</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -7132,10 +7132,10 @@
         <v>890</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49">
         <v>5</v>
@@ -7218,10 +7218,10 @@
         <v>890</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I50">
         <v>5</v>
@@ -7304,10 +7304,10 @@
         <v>890</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51">
         <v>5</v>
@@ -7390,10 +7390,10 @@
         <v>890</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I52">
         <v>5</v>
@@ -7479,7 +7479,7 @@
         <v>3</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I53">
         <v>5</v>
@@ -7565,7 +7565,7 @@
         <v>3</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I54">
         <v>5</v>
@@ -7648,10 +7648,10 @@
         <v>890</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I55">
         <v>5</v>
@@ -7734,10 +7734,10 @@
         <v>890</v>
       </c>
       <c r="G56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I56">
         <v>5</v>
@@ -7820,10 +7820,10 @@
         <v>890</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57">
         <v>5</v>
@@ -7906,10 +7906,10 @@
         <v>890</v>
       </c>
       <c r="G58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -8164,10 +8164,10 @@
         <v>890</v>
       </c>
       <c r="G61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I61">
         <v>5</v>
@@ -8250,10 +8250,10 @@
         <v>890</v>
       </c>
       <c r="G62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I62">
         <v>5</v>
@@ -8336,10 +8336,10 @@
         <v>890</v>
       </c>
       <c r="G63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I63">
         <v>5</v>
@@ -8422,10 +8422,10 @@
         <v>890</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I64">
         <v>5</v>
@@ -8508,10 +8508,10 @@
         <v>890</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I65">
         <v>5</v>
@@ -8594,10 +8594,10 @@
         <v>890</v>
       </c>
       <c r="G66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I66">
         <v>5</v>
@@ -8766,7 +8766,7 @@
         <v>890</v>
       </c>
       <c r="G68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -8852,7 +8852,7 @@
         <v>890</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H69">
         <v>2</v>
@@ -8938,7 +8938,7 @@
         <v>890</v>
       </c>
       <c r="G70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H70">
         <v>2</v>
@@ -9101,7 +9101,7 @@
         <v>890</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -9187,7 +9187,7 @@
         <v>890</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -9273,10 +9273,10 @@
         <v>890</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I74">
         <v>5</v>
@@ -9356,10 +9356,10 @@
         <v>890</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I75">
         <v>5</v>
@@ -9442,10 +9442,10 @@
         <v>890</v>
       </c>
       <c r="G76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I76">
         <v>5</v>
@@ -9617,7 +9617,7 @@
         <v>2</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I78">
         <v>5</v>
@@ -9789,7 +9789,7 @@
         <v>1</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I80">
         <v>5</v>
@@ -9955,10 +9955,10 @@
         <v>890</v>
       </c>
       <c r="G82">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82">
         <v>1</v>
@@ -10385,7 +10385,7 @@
         <v>890</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -10471,10 +10471,10 @@
         <v>890</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I88">
         <v>5</v>
@@ -10643,7 +10643,7 @@
         <v>3</v>
       </c>
       <c r="H90">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I90">
         <v>5</v>
@@ -10729,7 +10729,7 @@
         <v>1</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I91">
         <v>5</v>
@@ -10815,7 +10815,7 @@
         <v>1</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I92">
         <v>5</v>
@@ -10901,7 +10901,7 @@
         <v>1</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I93">
         <v>5</v>
@@ -10984,7 +10984,7 @@
         <v>1</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I94">
         <v>5</v>
@@ -11067,7 +11067,7 @@
         <v>1</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I95">
         <v>5</v>
@@ -11150,7 +11150,7 @@
         <v>2</v>
       </c>
       <c r="H96">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I96">
         <v>5</v>
@@ -11319,10 +11319,10 @@
         <v>890</v>
       </c>
       <c r="G98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I98">
         <v>5</v>
@@ -11405,10 +11405,10 @@
         <v>890</v>
       </c>
       <c r="G99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I99">
         <v>5</v>
@@ -11491,7 +11491,7 @@
         <v>890</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -11577,10 +11577,10 @@
         <v>890</v>
       </c>
       <c r="G101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I101">
         <v>5</v>
@@ -11663,10 +11663,10 @@
         <v>890</v>
       </c>
       <c r="G102">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I102">
         <v>5</v>
@@ -12176,7 +12176,7 @@
         <v>2</v>
       </c>
       <c r="H108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I108">
         <v>5</v>
@@ -12259,10 +12259,10 @@
         <v>890</v>
       </c>
       <c r="G109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H109">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I109">
         <v>5</v>
@@ -12348,7 +12348,7 @@
         <v>2</v>
       </c>
       <c r="H110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I110">
         <v>5</v>
@@ -12520,7 +12520,7 @@
         <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112">
         <v>5</v>
@@ -12606,7 +12606,7 @@
         <v>1</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113">
         <v>5</v>
@@ -12692,7 +12692,7 @@
         <v>1</v>
       </c>
       <c r="H114">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I114">
         <v>5</v>
@@ -12778,7 +12778,7 @@
         <v>1</v>
       </c>
       <c r="H115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I115">
         <v>5</v>
@@ -13205,10 +13205,10 @@
         <v>890</v>
       </c>
       <c r="G120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I120">
         <v>5</v>
@@ -13291,10 +13291,10 @@
         <v>890</v>
       </c>
       <c r="G121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I121">
         <v>5</v>
@@ -13377,10 +13377,10 @@
         <v>890</v>
       </c>
       <c r="G122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I122">
         <v>5</v>
@@ -13463,10 +13463,10 @@
         <v>890</v>
       </c>
       <c r="G123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I123">
         <v>5</v>
@@ -13807,10 +13807,10 @@
         <v>890</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I127">
         <v>5</v>
@@ -13890,10 +13890,10 @@
         <v>890</v>
       </c>
       <c r="G128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I128">
         <v>5</v>
@@ -13976,7 +13976,7 @@
         <v>2</v>
       </c>
       <c r="H129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I129">
         <v>5</v>
@@ -14062,7 +14062,7 @@
         <v>1</v>
       </c>
       <c r="H130">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I130">
         <v>5</v>
@@ -14148,7 +14148,7 @@
         <v>1</v>
       </c>
       <c r="H131">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I131">
         <v>5</v>
@@ -14234,7 +14234,7 @@
         <v>1</v>
       </c>
       <c r="H132">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I132">
         <v>5</v>
@@ -14320,7 +14320,7 @@
         <v>1</v>
       </c>
       <c r="H133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I133">
         <v>5</v>
@@ -14489,10 +14489,10 @@
         <v>890</v>
       </c>
       <c r="G135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I135">
         <v>1</v>
@@ -14664,7 +14664,7 @@
         <v>1</v>
       </c>
       <c r="H137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I137">
         <v>5</v>
@@ -14747,7 +14747,7 @@
         <v>1</v>
       </c>
       <c r="H138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I138">
         <v>5</v>
@@ -14830,7 +14830,7 @@
         <v>1</v>
       </c>
       <c r="H139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I139">
         <v>5</v>
@@ -14910,10 +14910,10 @@
         <v>890</v>
       </c>
       <c r="G140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I140">
         <v>5</v>
@@ -14996,7 +14996,7 @@
         <v>890</v>
       </c>
       <c r="G141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H141">
         <v>1</v>
@@ -15082,7 +15082,7 @@
         <v>890</v>
       </c>
       <c r="G142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H142">
         <v>1</v>
@@ -15168,7 +15168,7 @@
         <v>890</v>
       </c>
       <c r="G143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H143">
         <v>1</v>
@@ -15254,7 +15254,7 @@
         <v>890</v>
       </c>
       <c r="G144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H144">
         <v>1</v>
@@ -15343,7 +15343,7 @@
         <v>1</v>
       </c>
       <c r="H145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I145">
         <v>5</v>
@@ -15770,10 +15770,10 @@
         <v>890</v>
       </c>
       <c r="G150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I150">
         <v>1</v>
@@ -15856,10 +15856,10 @@
         <v>890</v>
       </c>
       <c r="G151">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H151">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I151">
         <v>5</v>
@@ -15945,7 +15945,7 @@
         <v>1</v>
       </c>
       <c r="H152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I152">
         <v>5</v>
@@ -16028,7 +16028,7 @@
         <v>1</v>
       </c>
       <c r="H153">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I153">
         <v>5</v>
@@ -16114,7 +16114,7 @@
         <v>1</v>
       </c>
       <c r="H154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I154">
         <v>5</v>
@@ -16286,7 +16286,7 @@
         <v>1</v>
       </c>
       <c r="H156">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I156">
         <v>5</v>
@@ -16366,7 +16366,7 @@
         <v>890</v>
       </c>
       <c r="G157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H157">
         <v>1</v>
@@ -16627,7 +16627,7 @@
         <v>1</v>
       </c>
       <c r="H160">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I160">
         <v>5</v>
@@ -16882,7 +16882,7 @@
         <v>1</v>
       </c>
       <c r="H163">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I163">
         <v>5</v>
@@ -17051,10 +17051,10 @@
         <v>890</v>
       </c>
       <c r="G165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I165">
         <v>5</v>
@@ -17315,7 +17315,7 @@
         <v>1</v>
       </c>
       <c r="H168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I168">
         <v>5</v>
@@ -17395,10 +17395,10 @@
         <v>890</v>
       </c>
       <c r="G169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I169">
         <v>5</v>
@@ -17484,7 +17484,7 @@
         <v>3</v>
       </c>
       <c r="H170">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I170">
         <v>5</v>
@@ -17653,10 +17653,10 @@
         <v>890</v>
       </c>
       <c r="G172">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H172">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I172">
         <v>5</v>
@@ -17739,10 +17739,10 @@
         <v>890</v>
       </c>
       <c r="G173">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H173">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I173">
         <v>5</v>
@@ -18599,10 +18599,10 @@
         <v>890</v>
       </c>
       <c r="G183">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H183">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I183">
         <v>5</v>
@@ -19029,10 +19029,10 @@
         <v>890</v>
       </c>
       <c r="G188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I188">
         <v>5</v>
@@ -19115,7 +19115,7 @@
         <v>3</v>
       </c>
       <c r="H189">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I189">
         <v>1</v>
@@ -19803,7 +19803,7 @@
         <v>3</v>
       </c>
       <c r="H197">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I197">
         <v>5</v>
@@ -19889,7 +19889,7 @@
         <v>3</v>
       </c>
       <c r="H198">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I198">
         <v>1</v>
@@ -20316,10 +20316,10 @@
         <v>890</v>
       </c>
       <c r="G203">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H203">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I203">
         <v>5</v>
@@ -20402,7 +20402,7 @@
         <v>3</v>
       </c>
       <c r="H204">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I204">
         <v>5</v>
@@ -20488,7 +20488,7 @@
         <v>3</v>
       </c>
       <c r="H205">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I205">
         <v>5</v>
@@ -20656,12 +20656,6 @@
       <c r="F207" t="s">
         <v>890</v>
       </c>
-      <c r="G207" t="s">
-        <v>892</v>
-      </c>
-      <c r="H207">
-        <v>2</v>
-      </c>
       <c r="I207">
         <v>5</v>
       </c>
@@ -20697,12 +20691,6 @@
       <c r="F208" t="s">
         <v>890</v>
       </c>
-      <c r="G208" t="s">
-        <v>892</v>
-      </c>
-      <c r="H208">
-        <v>2</v>
-      </c>
       <c r="I208">
         <v>5</v>
       </c>
@@ -20847,12 +20835,6 @@
       <c r="F211" t="s">
         <v>890</v>
       </c>
-      <c r="G211" t="s">
-        <v>892</v>
-      </c>
-      <c r="H211">
-        <v>1</v>
-      </c>
       <c r="I211">
         <v>5</v>
       </c>
@@ -20888,12 +20870,6 @@
       <c r="F212" t="s">
         <v>890</v>
       </c>
-      <c r="G212" t="s">
-        <v>892</v>
-      </c>
-      <c r="H212">
-        <v>1</v>
-      </c>
       <c r="I212">
         <v>1</v>
       </c>
@@ -20929,12 +20905,6 @@
       <c r="F213" t="s">
         <v>890</v>
       </c>
-      <c r="G213" t="s">
-        <v>892</v>
-      </c>
-      <c r="H213">
-        <v>1</v>
-      </c>
       <c r="I213">
         <v>5</v>
       </c>
@@ -20970,12 +20940,6 @@
       <c r="F214" t="s">
         <v>890</v>
       </c>
-      <c r="G214" t="s">
-        <v>892</v>
-      </c>
-      <c r="H214">
-        <v>1</v>
-      </c>
       <c r="I214">
         <v>5</v>
       </c>
@@ -21011,12 +20975,6 @@
       <c r="F215" t="s">
         <v>890</v>
       </c>
-      <c r="G215" t="s">
-        <v>892</v>
-      </c>
-      <c r="H215">
-        <v>1</v>
-      </c>
       <c r="I215">
         <v>5</v>
       </c>
@@ -21052,12 +21010,6 @@
       <c r="F216" t="s">
         <v>890</v>
       </c>
-      <c r="G216" t="s">
-        <v>892</v>
-      </c>
-      <c r="H216">
-        <v>1</v>
-      </c>
       <c r="I216">
         <v>5</v>
       </c>
@@ -21340,10 +21292,10 @@
         <v>890</v>
       </c>
       <c r="G223">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H223">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I223">
         <v>5</v>
@@ -21381,10 +21333,10 @@
         <v>890</v>
       </c>
       <c r="G224">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H224">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I224">
         <v>5</v>
@@ -21443,7 +21395,7 @@
         <v>3</v>
       </c>
       <c r="H225">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I225">
         <v>1</v>
@@ -21484,7 +21436,7 @@
         <v>892</v>
       </c>
       <c r="H226">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I226">
         <v>5</v>
@@ -21525,7 +21477,7 @@
         <v>892</v>
       </c>
       <c r="H227">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I227">
         <v>1</v>
@@ -21566,7 +21518,7 @@
         <v>892</v>
       </c>
       <c r="H228">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I228">
         <v>1</v>
@@ -21607,7 +21559,7 @@
         <v>892</v>
       </c>
       <c r="H229">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I229">
         <v>5</v>
@@ -21648,7 +21600,7 @@
         <v>892</v>
       </c>
       <c r="H230">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I230">
         <v>5</v>
@@ -21727,7 +21679,7 @@
         <v>890</v>
       </c>
       <c r="G232">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H232">
         <v>1</v>
@@ -21786,7 +21738,7 @@
         <v>890</v>
       </c>
       <c r="G233">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H233">
         <v>1</v>
@@ -21845,7 +21797,7 @@
         <v>890</v>
       </c>
       <c r="G234">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H234">
         <v>1</v>
@@ -21886,7 +21838,7 @@
         <v>890</v>
       </c>
       <c r="G235">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H235">
         <v>1</v>
@@ -21930,7 +21882,7 @@
         <v>892</v>
       </c>
       <c r="H236">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I236">
         <v>5</v>
@@ -21971,7 +21923,7 @@
         <v>892</v>
       </c>
       <c r="H237">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I237">
         <v>1</v>
@@ -22012,7 +21964,7 @@
         <v>892</v>
       </c>
       <c r="H238">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I238">
         <v>1</v>
@@ -22053,7 +22005,7 @@
         <v>892</v>
       </c>
       <c r="H239">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I239">
         <v>1</v>
@@ -22094,7 +22046,7 @@
         <v>3</v>
       </c>
       <c r="H240">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I240">
         <v>5</v>
@@ -22131,12 +22083,6 @@
       <c r="F241" t="s">
         <v>890</v>
       </c>
-      <c r="G241" t="s">
-        <v>892</v>
-      </c>
-      <c r="H241">
-        <v>2</v>
-      </c>
       <c r="I241">
         <v>5</v>
       </c>
@@ -22173,10 +22119,10 @@
         <v>890</v>
       </c>
       <c r="G242">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H242">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I242">
         <v>5</v>
@@ -22217,7 +22163,7 @@
         <v>1</v>
       </c>
       <c r="H243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I243">
         <v>5</v>
@@ -22258,7 +22204,7 @@
         <v>1</v>
       </c>
       <c r="H244">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I244">
         <v>5</v>
@@ -22378,7 +22324,7 @@
         <v>891</v>
       </c>
       <c r="G247">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H247">
         <v>3</v>
@@ -22463,7 +22409,7 @@
         <v>3</v>
       </c>
       <c r="H249">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I249">
         <v>5</v>
@@ -22504,7 +22450,7 @@
         <v>3</v>
       </c>
       <c r="H250">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I250">
         <v>5</v>
@@ -22545,7 +22491,7 @@
         <v>3</v>
       </c>
       <c r="H251">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I251">
         <v>5</v>
@@ -22586,7 +22532,7 @@
         <v>3</v>
       </c>
       <c r="H252">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I252">
         <v>5</v>
@@ -22627,7 +22573,7 @@
         <v>3</v>
       </c>
       <c r="H253">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I253">
         <v>1</v>
@@ -22668,7 +22614,7 @@
         <v>3</v>
       </c>
       <c r="H254">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I254">
         <v>1</v>
@@ -22706,7 +22652,7 @@
         <v>3</v>
       </c>
       <c r="H255">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I255">
         <v>1</v>
@@ -22747,7 +22693,7 @@
         <v>2</v>
       </c>
       <c r="H256">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I256">
         <v>5</v>
@@ -22870,7 +22816,7 @@
         <v>2</v>
       </c>
       <c r="H259">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I259">
         <v>5</v>
@@ -22911,7 +22857,7 @@
         <v>2</v>
       </c>
       <c r="H260">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I260">
         <v>5</v>
@@ -22946,7 +22892,7 @@
         <v>2</v>
       </c>
       <c r="H261">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I261">
         <v>5</v>
@@ -22984,10 +22930,10 @@
         <v>890</v>
       </c>
       <c r="G262">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H262">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I262">
         <v>5</v>
@@ -23025,10 +22971,10 @@
         <v>890</v>
       </c>
       <c r="G263">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H263">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I263">
         <v>5</v>
@@ -23066,10 +23012,10 @@
         <v>890</v>
       </c>
       <c r="G264">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H264">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I264">
         <v>5</v>
@@ -23306,7 +23252,7 @@
         <v>890</v>
       </c>
       <c r="G270">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H270">
         <v>2</v>
@@ -23347,7 +23293,7 @@
         <v>890</v>
       </c>
       <c r="G271">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H271">
         <v>2</v>
@@ -23388,7 +23334,7 @@
         <v>890</v>
       </c>
       <c r="G272">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H272">
         <v>2</v>
@@ -23429,7 +23375,7 @@
         <v>890</v>
       </c>
       <c r="G273">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H273">
         <v>2</v>
@@ -23470,7 +23416,7 @@
         <v>891</v>
       </c>
       <c r="G274">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H274">
         <v>2</v>
@@ -23511,7 +23457,7 @@
         <v>890</v>
       </c>
       <c r="G275">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H275">
         <v>3</v>
@@ -23902,7 +23848,7 @@
         <v>890</v>
       </c>
       <c r="G283">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H283">
         <v>2</v>
@@ -23961,7 +23907,7 @@
         <v>890</v>
       </c>
       <c r="G284">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H284">
         <v>2</v>
@@ -24002,7 +23948,7 @@
         <v>890</v>
       </c>
       <c r="G285">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H285">
         <v>2</v>
@@ -24043,7 +23989,7 @@
         <v>890</v>
       </c>
       <c r="G286">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H286">
         <v>2</v>
@@ -24084,7 +24030,7 @@
         <v>890</v>
       </c>
       <c r="G287">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H287">
         <v>3</v>
@@ -24125,7 +24071,7 @@
         <v>890</v>
       </c>
       <c r="G288">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H288">
         <v>3</v>
@@ -24166,7 +24112,7 @@
         <v>890</v>
       </c>
       <c r="G289">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H289">
         <v>3</v>
@@ -24207,7 +24153,7 @@
         <v>890</v>
       </c>
       <c r="G290">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H290">
         <v>3</v>
@@ -24248,7 +24194,7 @@
         <v>890</v>
       </c>
       <c r="G291">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H291">
         <v>3</v>
@@ -24289,7 +24235,7 @@
         <v>890</v>
       </c>
       <c r="G292">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H292">
         <v>3</v>
@@ -24330,10 +24276,10 @@
         <v>890</v>
       </c>
       <c r="G293">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H293">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I293">
         <v>5</v>
@@ -24371,10 +24317,10 @@
         <v>890</v>
       </c>
       <c r="G294">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H294">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I294">
         <v>5</v>
@@ -24412,10 +24358,10 @@
         <v>890</v>
       </c>
       <c r="G295">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H295">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I295">
         <v>5</v>
@@ -24453,10 +24399,10 @@
         <v>890</v>
       </c>
       <c r="G296">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H296">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I296">
         <v>5</v>
@@ -24494,10 +24440,10 @@
         <v>890</v>
       </c>
       <c r="G297">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H297">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I297">
         <v>5</v>
@@ -24535,10 +24481,10 @@
         <v>890</v>
       </c>
       <c r="G298">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H298">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I298">
         <v>5</v>
@@ -24576,10 +24522,10 @@
         <v>890</v>
       </c>
       <c r="G299">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H299">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I299">
         <v>5</v>
@@ -24617,10 +24563,10 @@
         <v>890</v>
       </c>
       <c r="G300">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H300">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I300">
         <v>5</v>
@@ -24658,10 +24604,10 @@
         <v>891</v>
       </c>
       <c r="G301">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H301">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I301">
         <v>5</v>
@@ -24881,10 +24827,10 @@
         <v>890</v>
       </c>
       <c r="G306">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H306">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I306">
         <v>5</v>
@@ -24922,10 +24868,10 @@
         <v>890</v>
       </c>
       <c r="G307">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H307">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I307">
         <v>1</v>
@@ -24963,10 +24909,10 @@
         <v>890</v>
       </c>
       <c r="G308">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H308">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I308">
         <v>1</v>
@@ -25007,7 +24953,7 @@
         <v>3</v>
       </c>
       <c r="H309">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I309">
         <v>5</v>
@@ -25045,10 +24991,10 @@
         <v>891</v>
       </c>
       <c r="G310">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H310">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I310">
         <v>5</v>
@@ -25086,10 +25032,10 @@
         <v>890</v>
       </c>
       <c r="G311">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H311">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I311">
         <v>5</v>
@@ -25127,10 +25073,10 @@
         <v>890</v>
       </c>
       <c r="G312">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H312">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I312">
         <v>1</v>
@@ -25168,10 +25114,10 @@
         <v>890</v>
       </c>
       <c r="G313">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H313">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I313">
         <v>1</v>
@@ -25253,7 +25199,7 @@
         <v>1</v>
       </c>
       <c r="H315">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I315">
         <v>5</v>
@@ -25335,7 +25281,7 @@
         <v>3</v>
       </c>
       <c r="H317">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I317">
         <v>5</v>
@@ -25947,7 +25893,7 @@
         <v>890</v>
       </c>
       <c r="G332">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H332">
         <v>1</v>
@@ -25988,7 +25934,7 @@
         <v>890</v>
       </c>
       <c r="G333">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H333">
         <v>1</v>
@@ -26029,7 +25975,7 @@
         <v>890</v>
       </c>
       <c r="G334">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H334">
         <v>1</v>
@@ -26287,7 +26233,7 @@
         <v>890</v>
       </c>
       <c r="G340">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H340">
         <v>2</v>
@@ -26328,7 +26274,7 @@
         <v>890</v>
       </c>
       <c r="G341">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H341">
         <v>2</v>
@@ -26454,7 +26400,7 @@
         <v>2</v>
       </c>
       <c r="H344">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I344">
         <v>5</v>
@@ -26574,10 +26520,10 @@
         <v>890</v>
       </c>
       <c r="G347">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H347">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I347">
         <v>5</v>
@@ -26615,10 +26561,10 @@
         <v>890</v>
       </c>
       <c r="G348">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H348">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I348">
         <v>5</v>
@@ -26656,10 +26602,10 @@
         <v>890</v>
       </c>
       <c r="G349">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H349">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I349">
         <v>5</v>
@@ -26697,10 +26643,10 @@
         <v>890</v>
       </c>
       <c r="G350">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H350">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I350">
         <v>1</v>
@@ -26738,10 +26684,10 @@
         <v>890</v>
       </c>
       <c r="G351">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H351">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I351">
         <v>1</v>
@@ -26779,10 +26725,10 @@
         <v>890</v>
       </c>
       <c r="G352">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H352">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I352">
         <v>1</v>
@@ -27189,10 +27135,10 @@
         <v>890</v>
       </c>
       <c r="G362">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H362">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I362">
         <v>5</v>
@@ -27696,10 +27642,10 @@
         <v>890</v>
       </c>
       <c r="G374">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H374">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I374">
         <v>5</v>
@@ -27737,10 +27683,10 @@
         <v>890</v>
       </c>
       <c r="G375">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H375">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I375">
         <v>5</v>
@@ -27778,10 +27724,10 @@
         <v>890</v>
       </c>
       <c r="G376">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H376">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I376">
         <v>5</v>
@@ -27819,10 +27765,10 @@
         <v>890</v>
       </c>
       <c r="G377">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H377">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I377">
         <v>5</v>
@@ -27860,10 +27806,10 @@
         <v>890</v>
       </c>
       <c r="G378">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H378">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I378">
         <v>5</v>
@@ -27901,10 +27847,10 @@
         <v>890</v>
       </c>
       <c r="G379">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H379">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I379">
         <v>5</v>
@@ -28209,7 +28155,7 @@
         <v>2</v>
       </c>
       <c r="H386">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I386">
         <v>5</v>
@@ -28288,10 +28234,10 @@
         <v>890</v>
       </c>
       <c r="G388">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H388">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I388">
         <v>1</v>
@@ -28329,10 +28275,10 @@
         <v>890</v>
       </c>
       <c r="G389">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H389">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I389">
         <v>1</v>
@@ -28411,7 +28357,7 @@
         <v>890</v>
       </c>
       <c r="G391">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H391">
         <v>1</v>
@@ -28452,7 +28398,7 @@
         <v>890</v>
       </c>
       <c r="G392">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H392">
         <v>1</v>
@@ -28493,7 +28439,7 @@
         <v>890</v>
       </c>
       <c r="G393">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H393">
         <v>1</v>
@@ -28534,7 +28480,7 @@
         <v>890</v>
       </c>
       <c r="G394">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H394">
         <v>1</v>
@@ -28575,7 +28521,7 @@
         <v>890</v>
       </c>
       <c r="G395">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H395">
         <v>1</v>
@@ -28616,7 +28562,7 @@
         <v>891</v>
       </c>
       <c r="G396">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H396">
         <v>1</v>
@@ -28657,7 +28603,7 @@
         <v>891</v>
       </c>
       <c r="G397">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H397">
         <v>1</v>
@@ -28698,7 +28644,7 @@
         <v>891</v>
       </c>
       <c r="G398">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H398">
         <v>1</v>
@@ -29398,7 +29344,7 @@
         <v>3</v>
       </c>
       <c r="H415">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I415">
         <v>1</v>
@@ -29599,12 +29545,6 @@
       <c r="F420" t="s">
         <v>890</v>
       </c>
-      <c r="G420" t="s">
-        <v>892</v>
-      </c>
-      <c r="H420">
-        <v>1</v>
-      </c>
       <c r="I420">
         <v>5</v>
       </c>
@@ -29640,12 +29580,6 @@
       <c r="F421" t="s">
         <v>890</v>
       </c>
-      <c r="G421" t="s">
-        <v>892</v>
-      </c>
-      <c r="H421">
-        <v>1</v>
-      </c>
       <c r="I421">
         <v>5</v>
       </c>
@@ -29681,12 +29615,6 @@
       <c r="F422" t="s">
         <v>890</v>
       </c>
-      <c r="G422" t="s">
-        <v>892</v>
-      </c>
-      <c r="H422">
-        <v>1</v>
-      </c>
       <c r="I422">
         <v>5</v>
       </c>
@@ -29722,12 +29650,6 @@
       <c r="F423" t="s">
         <v>890</v>
       </c>
-      <c r="G423" t="s">
-        <v>892</v>
-      </c>
-      <c r="H423">
-        <v>1</v>
-      </c>
       <c r="I423">
         <v>5</v>
       </c>
@@ -29763,12 +29685,6 @@
       <c r="F424" t="s">
         <v>890</v>
       </c>
-      <c r="G424" t="s">
-        <v>892</v>
-      </c>
-      <c r="H424">
-        <v>1</v>
-      </c>
       <c r="I424">
         <v>5</v>
       </c>
@@ -29804,12 +29720,6 @@
       <c r="F425" t="s">
         <v>890</v>
       </c>
-      <c r="G425" t="s">
-        <v>892</v>
-      </c>
-      <c r="H425">
-        <v>1</v>
-      </c>
       <c r="I425">
         <v>5</v>
       </c>
@@ -29845,12 +29755,6 @@
       <c r="F426" t="s">
         <v>890</v>
       </c>
-      <c r="G426" t="s">
-        <v>892</v>
-      </c>
-      <c r="H426">
-        <v>1</v>
-      </c>
       <c r="I426">
         <v>5</v>
       </c>
@@ -29886,12 +29790,6 @@
       <c r="F427" t="s">
         <v>890</v>
       </c>
-      <c r="G427" t="s">
-        <v>892</v>
-      </c>
-      <c r="H427">
-        <v>1</v>
-      </c>
       <c r="I427">
         <v>5</v>
       </c>
@@ -29972,7 +29870,7 @@
         <v>3</v>
       </c>
       <c r="H429">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I429">
         <v>1</v>
@@ -30054,7 +29952,7 @@
         <v>2</v>
       </c>
       <c r="H431">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I431">
         <v>5</v>
@@ -30095,7 +29993,7 @@
         <v>2</v>
       </c>
       <c r="H432">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I432">
         <v>5</v>
@@ -30136,7 +30034,7 @@
         <v>2</v>
       </c>
       <c r="H433">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I433">
         <v>1</v>
@@ -30177,7 +30075,7 @@
         <v>2</v>
       </c>
       <c r="H434">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I434">
         <v>5</v>
@@ -30218,7 +30116,7 @@
         <v>892</v>
       </c>
       <c r="H435">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I435">
         <v>1</v>
@@ -30256,7 +30154,7 @@
         <v>2</v>
       </c>
       <c r="H436">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I436">
         <v>5</v>
@@ -30991,7 +30889,7 @@
         <v>890</v>
       </c>
       <c r="G454">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H454">
         <v>3</v>
@@ -31073,10 +30971,10 @@
         <v>890</v>
       </c>
       <c r="G456">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H456">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I456">
         <v>1</v>
@@ -31114,10 +31012,10 @@
         <v>890</v>
       </c>
       <c r="G457">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H457">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I457">
         <v>5</v>
@@ -31155,10 +31053,10 @@
         <v>890</v>
       </c>
       <c r="G458">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H458">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I458">
         <v>5</v>
@@ -31196,10 +31094,10 @@
         <v>890</v>
       </c>
       <c r="G459">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H459">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I459">
         <v>5</v>
@@ -31237,10 +31135,10 @@
         <v>890</v>
       </c>
       <c r="G460">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H460">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I460">
         <v>5</v>
@@ -31278,10 +31176,10 @@
         <v>891</v>
       </c>
       <c r="G461">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H461">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I461">
         <v>5</v>
@@ -31442,10 +31340,10 @@
         <v>891</v>
       </c>
       <c r="G465">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H465">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I465">
         <v>5</v>
@@ -31851,12 +31749,6 @@
       <c r="F475" t="s">
         <v>890</v>
       </c>
-      <c r="G475" t="s">
-        <v>892</v>
-      </c>
-      <c r="H475">
-        <v>1</v>
-      </c>
       <c r="I475">
         <v>5</v>
       </c>
@@ -31998,10 +31890,10 @@
         <v>890</v>
       </c>
       <c r="G479">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H479">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I479">
         <v>1</v>
@@ -32039,10 +31931,10 @@
         <v>890</v>
       </c>
       <c r="G480">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H480">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I480">
         <v>1</v>
@@ -32080,10 +31972,10 @@
         <v>890</v>
       </c>
       <c r="G481">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H481">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I481">
         <v>1</v>
@@ -32121,10 +32013,10 @@
         <v>890</v>
       </c>
       <c r="G482">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H482">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I482">
         <v>1</v>
@@ -32162,10 +32054,10 @@
         <v>890</v>
       </c>
       <c r="G483">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H483">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I483">
         <v>5</v>
@@ -32203,10 +32095,10 @@
         <v>890</v>
       </c>
       <c r="G484">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H484">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I484">
         <v>1</v>
@@ -32449,7 +32341,7 @@
         <v>890</v>
       </c>
       <c r="G490">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H490">
         <v>3</v>
@@ -32490,10 +32382,10 @@
         <v>890</v>
       </c>
       <c r="G491">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H491">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I491">
         <v>5</v>
@@ -32695,7 +32587,7 @@
         <v>890</v>
       </c>
       <c r="G496">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H496">
         <v>2</v>
@@ -32780,7 +32672,7 @@
         <v>2</v>
       </c>
       <c r="H498">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I498">
         <v>5</v>
@@ -32821,7 +32713,7 @@
         <v>2</v>
       </c>
       <c r="H499">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I499">
         <v>1</v>
@@ -32941,10 +32833,10 @@
         <v>890</v>
       </c>
       <c r="G502">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H502">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I502">
         <v>5</v>
@@ -32982,10 +32874,10 @@
         <v>890</v>
       </c>
       <c r="G503">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H503">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I503">
         <v>5</v>
@@ -33023,10 +32915,10 @@
         <v>890</v>
       </c>
       <c r="G504">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H504">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I504">
         <v>5</v>
@@ -33064,10 +32956,10 @@
         <v>890</v>
       </c>
       <c r="G505">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H505">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I505">
         <v>5</v>
@@ -33105,10 +32997,10 @@
         <v>890</v>
       </c>
       <c r="G506">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H506">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I506">
         <v>5</v>
@@ -33146,10 +33038,10 @@
         <v>890</v>
       </c>
       <c r="G507">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H507">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I507">
         <v>5</v>
@@ -33187,10 +33079,10 @@
         <v>890</v>
       </c>
       <c r="G508">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H508">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I508">
         <v>5</v>
@@ -33392,10 +33284,10 @@
         <v>890</v>
       </c>
       <c r="G513">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H513">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I513">
         <v>5</v>
@@ -33430,10 +33322,10 @@
         <v>890</v>
       </c>
       <c r="G514">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H514">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I514">
         <v>1</v>
@@ -33471,7 +33363,7 @@
         <v>890</v>
       </c>
       <c r="G515">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H515">
         <v>3</v>
@@ -33512,7 +33404,7 @@
         <v>890</v>
       </c>
       <c r="G516">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H516">
         <v>3</v>
@@ -34053,7 +33945,7 @@
         <v>890</v>
       </c>
       <c r="G530">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H530">
         <v>2</v>
@@ -34160,12 +34052,6 @@
       <c r="F533" t="s">
         <v>890</v>
       </c>
-      <c r="G533" t="s">
-        <v>892</v>
-      </c>
-      <c r="H533">
-        <v>2</v>
-      </c>
       <c r="I533">
         <v>5</v>
       </c>
@@ -34201,12 +34087,6 @@
       <c r="F534" t="s">
         <v>890</v>
       </c>
-      <c r="G534" t="s">
-        <v>892</v>
-      </c>
-      <c r="H534">
-        <v>2</v>
-      </c>
       <c r="I534">
         <v>5</v>
       </c>
@@ -34242,12 +34122,6 @@
       <c r="F535" t="s">
         <v>890</v>
       </c>
-      <c r="G535" t="s">
-        <v>892</v>
-      </c>
-      <c r="H535">
-        <v>2</v>
-      </c>
       <c r="I535">
         <v>5</v>
       </c>
@@ -34283,12 +34157,6 @@
       <c r="F536" t="s">
         <v>890</v>
       </c>
-      <c r="G536" t="s">
-        <v>892</v>
-      </c>
-      <c r="H536">
-        <v>2</v>
-      </c>
       <c r="I536">
         <v>5</v>
       </c>
@@ -34321,12 +34189,6 @@
       <c r="F537" t="s">
         <v>890</v>
       </c>
-      <c r="G537" t="s">
-        <v>892</v>
-      </c>
-      <c r="H537">
-        <v>2</v>
-      </c>
       <c r="I537">
         <v>5</v>
       </c>
@@ -34362,12 +34224,6 @@
       <c r="F538" t="s">
         <v>890</v>
       </c>
-      <c r="G538" t="s">
-        <v>892</v>
-      </c>
-      <c r="H538">
-        <v>2</v>
-      </c>
       <c r="I538">
         <v>5</v>
       </c>
@@ -34403,12 +34259,6 @@
       <c r="F539" t="s">
         <v>890</v>
       </c>
-      <c r="G539" t="s">
-        <v>892</v>
-      </c>
-      <c r="H539">
-        <v>2</v>
-      </c>
       <c r="I539">
         <v>5</v>
       </c>
@@ -36442,7 +36292,7 @@
         <v>890</v>
       </c>
       <c r="G598">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H598">
         <v>3</v>
@@ -36486,7 +36336,7 @@
         <v>1</v>
       </c>
       <c r="H599">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I599">
         <v>5</v>
@@ -36524,7 +36374,7 @@
         <v>890</v>
       </c>
       <c r="G600">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H600">
         <v>2</v>
@@ -36565,7 +36415,7 @@
         <v>890</v>
       </c>
       <c r="G601">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H601">
         <v>2</v>
@@ -36606,7 +36456,7 @@
         <v>890</v>
       </c>
       <c r="G602">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H602">
         <v>2</v>
@@ -36647,7 +36497,7 @@
         <v>890</v>
       </c>
       <c r="G603">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H603">
         <v>2</v>
@@ -36688,7 +36538,7 @@
         <v>890</v>
       </c>
       <c r="G604">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H604">
         <v>2</v>
@@ -36729,7 +36579,7 @@
         <v>890</v>
       </c>
       <c r="G605">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H605">
         <v>2</v>
@@ -36770,7 +36620,7 @@
         <v>890</v>
       </c>
       <c r="G606">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H606">
         <v>2</v>
@@ -36811,7 +36661,7 @@
         <v>890</v>
       </c>
       <c r="G607">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H607">
         <v>2</v>
@@ -36852,7 +36702,7 @@
         <v>890</v>
       </c>
       <c r="G608">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H608">
         <v>2</v>
@@ -36893,7 +36743,7 @@
         <v>890</v>
       </c>
       <c r="G609">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H609">
         <v>3</v>
@@ -36934,7 +36784,7 @@
         <v>890</v>
       </c>
       <c r="G610">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H610">
         <v>3</v>
@@ -37048,7 +36898,7 @@
         <v>890</v>
       </c>
       <c r="G613">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H613">
         <v>1</v>
@@ -37297,7 +37147,7 @@
         <v>1</v>
       </c>
       <c r="H619">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I619">
         <v>5</v>
@@ -37376,7 +37226,7 @@
         <v>890</v>
       </c>
       <c r="G621">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H621">
         <v>2</v>
@@ -37991,7 +37841,7 @@
         <v>890</v>
       </c>
       <c r="G636">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H636">
         <v>3</v>
@@ -38032,7 +37882,7 @@
         <v>890</v>
       </c>
       <c r="G637">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H637">
         <v>3</v>
@@ -38073,7 +37923,7 @@
         <v>891</v>
       </c>
       <c r="G638">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H638">
         <v>3</v>
@@ -38114,7 +37964,7 @@
         <v>890</v>
       </c>
       <c r="G639">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H639">
         <v>2</v>
@@ -38154,12 +38004,6 @@
       <c r="F640" t="s">
         <v>890</v>
       </c>
-      <c r="G640" t="s">
-        <v>892</v>
-      </c>
-      <c r="H640">
-        <v>1</v>
-      </c>
       <c r="I640">
         <v>5</v>
       </c>
@@ -38195,12 +38039,6 @@
       <c r="F641" t="s">
         <v>890</v>
       </c>
-      <c r="G641" t="s">
-        <v>892</v>
-      </c>
-      <c r="H641">
-        <v>1</v>
-      </c>
       <c r="I641">
         <v>1</v>
       </c>
@@ -38236,12 +38074,6 @@
       <c r="F642" t="s">
         <v>890</v>
       </c>
-      <c r="G642" t="s">
-        <v>892</v>
-      </c>
-      <c r="H642">
-        <v>1</v>
-      </c>
       <c r="I642">
         <v>5</v>
       </c>
@@ -38277,12 +38109,6 @@
       <c r="F643" t="s">
         <v>890</v>
       </c>
-      <c r="G643" t="s">
-        <v>892</v>
-      </c>
-      <c r="H643">
-        <v>1</v>
-      </c>
       <c r="I643">
         <v>5</v>
       </c>
@@ -38318,12 +38144,6 @@
       <c r="F644" t="s">
         <v>890</v>
       </c>
-      <c r="G644" t="s">
-        <v>892</v>
-      </c>
-      <c r="H644">
-        <v>1</v>
-      </c>
       <c r="I644">
         <v>5</v>
       </c>
@@ -38359,12 +38179,6 @@
       <c r="F645" t="s">
         <v>890</v>
       </c>
-      <c r="G645" t="s">
-        <v>892</v>
-      </c>
-      <c r="H645">
-        <v>1</v>
-      </c>
       <c r="I645">
         <v>5</v>
       </c>
@@ -38400,12 +38214,6 @@
       <c r="F646" t="s">
         <v>890</v>
       </c>
-      <c r="G646" t="s">
-        <v>892</v>
-      </c>
-      <c r="H646">
-        <v>1</v>
-      </c>
       <c r="I646">
         <v>5</v>
       </c>
@@ -38441,12 +38249,6 @@
       <c r="F647" t="s">
         <v>890</v>
       </c>
-      <c r="G647" t="s">
-        <v>892</v>
-      </c>
-      <c r="H647">
-        <v>1</v>
-      </c>
       <c r="I647">
         <v>5</v>
       </c>
@@ -38482,12 +38284,6 @@
       <c r="F648" t="s">
         <v>890</v>
       </c>
-      <c r="G648" t="s">
-        <v>892</v>
-      </c>
-      <c r="H648">
-        <v>1</v>
-      </c>
       <c r="I648">
         <v>5</v>
       </c>
@@ -38523,12 +38319,6 @@
       <c r="F649" t="s">
         <v>890</v>
       </c>
-      <c r="G649" t="s">
-        <v>892</v>
-      </c>
-      <c r="H649">
-        <v>1</v>
-      </c>
       <c r="I649">
         <v>5</v>
       </c>
@@ -38564,12 +38354,6 @@
       <c r="F650" t="s">
         <v>890</v>
       </c>
-      <c r="G650" t="s">
-        <v>892</v>
-      </c>
-      <c r="H650">
-        <v>1</v>
-      </c>
       <c r="I650">
         <v>5</v>
       </c>
@@ -38605,12 +38389,6 @@
       <c r="F651" t="s">
         <v>890</v>
       </c>
-      <c r="G651" t="s">
-        <v>892</v>
-      </c>
-      <c r="H651">
-        <v>1</v>
-      </c>
       <c r="I651">
         <v>1</v>
       </c>
@@ -38646,12 +38424,6 @@
       <c r="F652" t="s">
         <v>890</v>
       </c>
-      <c r="G652" t="s">
-        <v>892</v>
-      </c>
-      <c r="H652">
-        <v>1</v>
-      </c>
       <c r="I652">
         <v>5</v>
       </c>
@@ -38811,7 +38583,7 @@
         <v>891</v>
       </c>
       <c r="G656">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H656">
         <v>3</v>
@@ -38924,12 +38696,6 @@
       <c r="F659" t="s">
         <v>890</v>
       </c>
-      <c r="G659" t="s">
-        <v>892</v>
-      </c>
-      <c r="H659">
-        <v>1</v>
-      </c>
       <c r="I659">
         <v>5</v>
       </c>
@@ -38965,12 +38731,6 @@
       <c r="F660" t="s">
         <v>890</v>
       </c>
-      <c r="G660" t="s">
-        <v>892</v>
-      </c>
-      <c r="H660">
-        <v>1</v>
-      </c>
       <c r="I660">
         <v>5</v>
       </c>
@@ -39003,12 +38763,6 @@
       <c r="F661" t="s">
         <v>890</v>
       </c>
-      <c r="G661" t="s">
-        <v>892</v>
-      </c>
-      <c r="H661">
-        <v>1</v>
-      </c>
       <c r="I661">
         <v>5</v>
       </c>
@@ -39044,12 +38798,6 @@
       <c r="F662" t="s">
         <v>890</v>
       </c>
-      <c r="G662" t="s">
-        <v>892</v>
-      </c>
-      <c r="H662">
-        <v>1</v>
-      </c>
       <c r="I662">
         <v>5</v>
       </c>
@@ -39085,12 +38833,6 @@
       <c r="F663" t="s">
         <v>890</v>
       </c>
-      <c r="G663" t="s">
-        <v>892</v>
-      </c>
-      <c r="H663">
-        <v>1</v>
-      </c>
       <c r="I663">
         <v>1</v>
       </c>
@@ -39126,12 +38868,6 @@
       <c r="F664" t="s">
         <v>891</v>
       </c>
-      <c r="G664" t="s">
-        <v>892</v>
-      </c>
-      <c r="H664">
-        <v>3</v>
-      </c>
       <c r="I664">
         <v>5</v>
       </c>
@@ -39168,7 +38904,7 @@
         <v>890</v>
       </c>
       <c r="G665">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H665">
         <v>2</v>
@@ -39209,7 +38945,7 @@
         <v>890</v>
       </c>
       <c r="G666">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H666">
         <v>2</v>
@@ -39250,7 +38986,7 @@
         <v>891</v>
       </c>
       <c r="G667">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H667">
         <v>2</v>
@@ -39291,7 +39027,7 @@
         <v>891</v>
       </c>
       <c r="G668">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H668">
         <v>2</v>
@@ -39537,10 +39273,10 @@
         <v>890</v>
       </c>
       <c r="G674">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H674">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I674">
         <v>5</v>
@@ -39888,10 +39624,10 @@
         <v>890</v>
       </c>
       <c r="G683">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H683">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I683">
         <v>5</v>
@@ -40084,7 +39820,7 @@
         <v>3</v>
       </c>
       <c r="H688">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I688">
         <v>1</v>
@@ -40125,7 +39861,7 @@
         <v>3</v>
       </c>
       <c r="H689">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I689">
         <v>1</v>
@@ -40166,7 +39902,7 @@
         <v>3</v>
       </c>
       <c r="H690">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I690">
         <v>1</v>
@@ -40207,7 +39943,7 @@
         <v>3</v>
       </c>
       <c r="H691">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I691">
         <v>1</v>
@@ -40320,12 +40056,6 @@
       <c r="F694" t="s">
         <v>890</v>
       </c>
-      <c r="G694" t="s">
-        <v>892</v>
-      </c>
-      <c r="H694">
-        <v>2</v>
-      </c>
       <c r="I694">
         <v>5</v>
       </c>
@@ -40397,7 +40127,7 @@
         <v>890</v>
       </c>
       <c r="G696">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H696">
         <v>2</v>
@@ -40438,7 +40168,7 @@
         <v>890</v>
       </c>
       <c r="G697">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H697">
         <v>2</v>
@@ -40479,7 +40209,7 @@
         <v>890</v>
       </c>
       <c r="G698">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H698">
         <v>2</v>
@@ -40683,12 +40413,6 @@
       <c r="F703" t="s">
         <v>890</v>
       </c>
-      <c r="G703" t="s">
-        <v>892</v>
-      </c>
-      <c r="H703">
-        <v>3</v>
-      </c>
       <c r="I703">
         <v>5</v>
       </c>
@@ -40765,12 +40489,6 @@
       <c r="F705" t="s">
         <v>890</v>
       </c>
-      <c r="G705" t="s">
-        <v>892</v>
-      </c>
-      <c r="H705">
-        <v>3</v>
-      </c>
       <c r="I705">
         <v>5</v>
       </c>
@@ -40806,12 +40524,6 @@
       <c r="F706" t="s">
         <v>890</v>
       </c>
-      <c r="G706" t="s">
-        <v>892</v>
-      </c>
-      <c r="H706">
-        <v>3</v>
-      </c>
       <c r="I706">
         <v>5</v>
       </c>
@@ -40847,12 +40559,6 @@
       <c r="F707" t="s">
         <v>890</v>
       </c>
-      <c r="G707" t="s">
-        <v>892</v>
-      </c>
-      <c r="H707">
-        <v>3</v>
-      </c>
       <c r="I707">
         <v>5</v>
       </c>
@@ -40892,7 +40598,7 @@
         <v>2</v>
       </c>
       <c r="H708">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I708">
         <v>5</v>
@@ -40933,7 +40639,7 @@
         <v>2</v>
       </c>
       <c r="H709">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I709">
         <v>5</v>
@@ -40974,7 +40680,7 @@
         <v>2</v>
       </c>
       <c r="H710">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I710">
         <v>1</v>
@@ -41015,7 +40721,7 @@
         <v>2</v>
       </c>
       <c r="H711">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I711">
         <v>5</v>
@@ -41056,7 +40762,7 @@
         <v>2</v>
       </c>
       <c r="H712">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I712">
         <v>5</v>
@@ -41097,7 +40803,7 @@
         <v>2</v>
       </c>
       <c r="H713">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I713">
         <v>5</v>
@@ -41176,7 +40882,7 @@
         <v>890</v>
       </c>
       <c r="G715">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H715">
         <v>3</v>
@@ -41217,7 +40923,7 @@
         <v>890</v>
       </c>
       <c r="G716">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H716">
         <v>3</v>
@@ -41258,7 +40964,7 @@
         <v>890</v>
       </c>
       <c r="G717">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H717">
         <v>3</v>
@@ -41299,7 +41005,7 @@
         <v>890</v>
       </c>
       <c r="G718">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H718">
         <v>3</v>
@@ -41340,7 +41046,7 @@
         <v>890</v>
       </c>
       <c r="G719">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H719">
         <v>3</v>
@@ -41381,7 +41087,7 @@
         <v>890</v>
       </c>
       <c r="G720">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H720">
         <v>3</v>
@@ -41422,7 +41128,7 @@
         <v>890</v>
       </c>
       <c r="G721">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H721">
         <v>3</v>
@@ -41463,7 +41169,7 @@
         <v>890</v>
       </c>
       <c r="G722">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H722">
         <v>3</v>
@@ -41504,7 +41210,7 @@
         <v>890</v>
       </c>
       <c r="G723">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H723">
         <v>3</v>
@@ -41545,7 +41251,7 @@
         <v>890</v>
       </c>
       <c r="G724">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H724">
         <v>3</v>
@@ -41589,7 +41295,7 @@
         <v>892</v>
       </c>
       <c r="H725">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I725">
         <v>5</v>
@@ -41626,12 +41332,6 @@
       <c r="F726" t="s">
         <v>891</v>
       </c>
-      <c r="G726" t="s">
-        <v>892</v>
-      </c>
-      <c r="H726">
-        <v>3</v>
-      </c>
       <c r="I726">
         <v>5</v>
       </c>
@@ -41667,12 +41367,6 @@
       <c r="F727" t="s">
         <v>891</v>
       </c>
-      <c r="G727" t="s">
-        <v>892</v>
-      </c>
-      <c r="H727">
-        <v>3</v>
-      </c>
       <c r="I727">
         <v>1</v>
       </c>
@@ -41708,12 +41402,6 @@
       <c r="F728" t="s">
         <v>891</v>
       </c>
-      <c r="G728" t="s">
-        <v>892</v>
-      </c>
-      <c r="H728">
-        <v>3</v>
-      </c>
       <c r="I728">
         <v>5</v>
       </c>
@@ -41749,12 +41437,6 @@
       <c r="F729" t="s">
         <v>891</v>
       </c>
-      <c r="G729" t="s">
-        <v>892</v>
-      </c>
-      <c r="H729">
-        <v>3</v>
-      </c>
       <c r="I729">
         <v>5</v>
       </c>
@@ -41787,12 +41469,6 @@
       <c r="F730" t="s">
         <v>891</v>
       </c>
-      <c r="G730" t="s">
-        <v>892</v>
-      </c>
-      <c r="H730">
-        <v>3</v>
-      </c>
       <c r="I730">
         <v>1</v>
       </c>
@@ -42154,7 +41830,7 @@
         <v>890</v>
       </c>
       <c r="G739">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H739">
         <v>3</v>
@@ -42195,7 +41871,7 @@
         <v>890</v>
       </c>
       <c r="G740">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H740">
         <v>3</v>

</xml_diff>